<commit_message>
update to track year closed
</commit_message>
<xml_diff>
--- a/data/raw/schools/2017-2018 Master School List (20180611).xlsx
+++ b/data/raw/schools/2017-2018 Master School List (20180611).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/DataVisualizations/asbestos-dashboard/asbestos-dashboard-data/data/raw/schools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754E4D59-3B18-D847-BAED-92F86636FDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA53008-31DA-4B4C-8691-E51E74CE800F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24000" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14819,11 +14819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:BE328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15048,7 +15047,7 @@
         <v>4467</v>
       </c>
     </row>
-    <row r="2" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -15221,7 +15220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -15394,7 +15393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -15567,7 +15566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -15740,7 +15739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -15913,7 +15912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -16086,7 +16085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -16259,7 +16258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -16432,7 +16431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -16605,7 +16604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -16778,7 +16777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -16951,7 +16950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -17124,7 +17123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -17297,7 +17296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -17470,7 +17469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -17643,7 +17642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -17816,7 +17815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -17989,7 +17988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -18162,7 +18161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -18335,7 +18334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -18508,7 +18507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -18681,7 +18680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -18854,7 +18853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -19027,7 +19026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -19200,7 +19199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
@@ -19373,7 +19372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -19546,7 +19545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -19719,7 +19718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
@@ -19892,7 +19891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
@@ -20065,7 +20064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
@@ -20238,7 +20237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>30</v>
       </c>
@@ -20411,7 +20410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -20584,7 +20583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
@@ -20757,7 +20756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -20930,7 +20929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
@@ -21103,7 +21102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
@@ -21276,7 +21275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>36</v>
       </c>
@@ -21449,7 +21448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
@@ -21622,7 +21621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
@@ -21795,7 +21794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>39</v>
       </c>
@@ -21968,7 +21967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
@@ -22141,7 +22140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
@@ -22314,7 +22313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
@@ -22487,7 +22486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -22660,7 +22659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>44</v>
       </c>
@@ -22833,7 +22832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>45</v>
       </c>
@@ -23006,7 +23005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>46</v>
       </c>
@@ -23179,7 +23178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>47</v>
       </c>
@@ -23352,7 +23351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>48</v>
       </c>
@@ -23525,7 +23524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>49</v>
       </c>
@@ -23698,7 +23697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>50</v>
       </c>
@@ -23871,7 +23870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>51</v>
       </c>
@@ -24044,7 +24043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>39</v>
       </c>
@@ -24217,7 +24216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>52</v>
       </c>
@@ -24390,7 +24389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>53</v>
       </c>
@@ -24563,7 +24562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
@@ -24736,7 +24735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>55</v>
       </c>
@@ -24909,7 +24908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
@@ -25082,7 +25081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>57</v>
       </c>
@@ -25255,7 +25254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -25428,7 +25427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
@@ -25601,7 +25600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>60</v>
       </c>
@@ -25774,7 +25773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
@@ -25947,7 +25946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>62</v>
       </c>
@@ -26120,7 +26119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>39</v>
       </c>
@@ -26293,7 +26292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>39</v>
       </c>
@@ -26466,7 +26465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>39</v>
       </c>
@@ -26639,7 +26638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>39</v>
       </c>
@@ -26812,7 +26811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>29</v>
       </c>
@@ -26985,7 +26984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>39</v>
       </c>
@@ -27158,7 +27157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>39</v>
       </c>
@@ -27331,7 +27330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>39</v>
       </c>
@@ -27504,7 +27503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>39</v>
       </c>
@@ -27677,7 +27676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>39</v>
       </c>
@@ -27850,7 +27849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>39</v>
       </c>
@@ -28023,7 +28022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>39</v>
       </c>
@@ -28196,7 +28195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>39</v>
       </c>
@@ -28369,7 +28368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>39</v>
       </c>
@@ -28542,7 +28541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>28</v>
       </c>
@@ -28715,7 +28714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>63</v>
       </c>
@@ -28888,7 +28887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>64</v>
       </c>
@@ -29061,7 +29060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>65</v>
       </c>
@@ -29234,7 +29233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>66</v>
       </c>
@@ -29407,7 +29406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>67</v>
       </c>
@@ -29580,7 +29579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>68</v>
       </c>
@@ -29753,7 +29752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>69</v>
       </c>
@@ -29926,7 +29925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>70</v>
       </c>
@@ -30099,7 +30098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>71</v>
       </c>
@@ -30272,7 +30271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>72</v>
       </c>
@@ -30445,7 +30444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>73</v>
       </c>
@@ -30618,7 +30617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>74</v>
       </c>
@@ -30791,7 +30790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>75</v>
       </c>
@@ -30964,7 +30963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>76</v>
       </c>
@@ -31137,7 +31136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>77</v>
       </c>
@@ -31310,7 +31309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>78</v>
       </c>
@@ -31483,7 +31482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>79</v>
       </c>
@@ -31656,7 +31655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>80</v>
       </c>
@@ -31829,7 +31828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>81</v>
       </c>
@@ -32002,7 +32001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>82</v>
       </c>
@@ -32175,7 +32174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>83</v>
       </c>
@@ -32348,7 +32347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>84</v>
       </c>
@@ -32521,7 +32520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>85</v>
       </c>
@@ -32694,7 +32693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>86</v>
       </c>
@@ -32867,7 +32866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>87</v>
       </c>
@@ -33040,7 +33039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>88</v>
       </c>
@@ -33213,7 +33212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>89</v>
       </c>
@@ -33386,7 +33385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>90</v>
       </c>
@@ -33559,7 +33558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>91</v>
       </c>
@@ -33732,7 +33731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>92</v>
       </c>
@@ -33905,7 +33904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>93</v>
       </c>
@@ -34078,7 +34077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>94</v>
       </c>
@@ -34251,7 +34250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>95</v>
       </c>
@@ -34424,7 +34423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>96</v>
       </c>
@@ -34597,7 +34596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>97</v>
       </c>
@@ -34770,7 +34769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>98</v>
       </c>
@@ -34943,7 +34942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>99</v>
       </c>
@@ -35116,7 +35115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>100</v>
       </c>
@@ -35289,7 +35288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>101</v>
       </c>
@@ -35635,7 +35634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>103</v>
       </c>
@@ -35808,7 +35807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>104</v>
       </c>
@@ -35981,7 +35980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>105</v>
       </c>
@@ -36154,7 +36153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>106</v>
       </c>
@@ -36327,7 +36326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>107</v>
       </c>
@@ -36500,7 +36499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>108</v>
       </c>
@@ -36673,7 +36672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>109</v>
       </c>
@@ -36846,7 +36845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>110</v>
       </c>
@@ -37019,7 +37018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>111</v>
       </c>
@@ -37192,7 +37191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>112</v>
       </c>
@@ -37365,7 +37364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>113</v>
       </c>
@@ -37538,7 +37537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>114</v>
       </c>
@@ -37711,7 +37710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>115</v>
       </c>
@@ -37884,7 +37883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>116</v>
       </c>
@@ -38057,7 +38056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>117</v>
       </c>
@@ -38230,7 +38229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>118</v>
       </c>
@@ -38403,7 +38402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>119</v>
       </c>
@@ -38576,7 +38575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>120</v>
       </c>
@@ -38749,7 +38748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>121</v>
       </c>
@@ -38922,7 +38921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>122</v>
       </c>
@@ -39095,7 +39094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>123</v>
       </c>
@@ -39268,7 +39267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>124</v>
       </c>
@@ -39441,7 +39440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>125</v>
       </c>
@@ -39614,7 +39613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>126</v>
       </c>
@@ -39787,7 +39786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>127</v>
       </c>
@@ -39960,7 +39959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>128</v>
       </c>
@@ -40133,7 +40132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>129</v>
       </c>
@@ -40306,7 +40305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>130</v>
       </c>
@@ -40479,7 +40478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>131</v>
       </c>
@@ -40652,7 +40651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>132</v>
       </c>
@@ -40825,7 +40824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>133</v>
       </c>
@@ -40998,7 +40997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>134</v>
       </c>
@@ -41171,7 +41170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>135</v>
       </c>
@@ -41344,7 +41343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>136</v>
       </c>
@@ -41517,7 +41516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>137</v>
       </c>
@@ -41690,7 +41689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>138</v>
       </c>
@@ -41863,7 +41862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>139</v>
       </c>
@@ -42036,7 +42035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>140</v>
       </c>
@@ -42209,7 +42208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>141</v>
       </c>
@@ -42382,7 +42381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>142</v>
       </c>
@@ -42555,7 +42554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>143</v>
       </c>
@@ -42728,7 +42727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>144</v>
       </c>
@@ -42901,7 +42900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>145</v>
       </c>
@@ -43074,7 +43073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>146</v>
       </c>
@@ -43247,7 +43246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>147</v>
       </c>
@@ -43420,7 +43419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>148</v>
       </c>
@@ -43593,7 +43592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>149</v>
       </c>
@@ -43766,7 +43765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>150</v>
       </c>
@@ -43939,7 +43938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>151</v>
       </c>
@@ -44112,7 +44111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>152</v>
       </c>
@@ -44285,7 +44284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>153</v>
       </c>
@@ -44458,7 +44457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>154</v>
       </c>
@@ -44631,7 +44630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>155</v>
       </c>
@@ -44804,7 +44803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>156</v>
       </c>
@@ -44977,7 +44976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>157</v>
       </c>
@@ -45150,7 +45149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>158</v>
       </c>
@@ -45323,7 +45322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>159</v>
       </c>
@@ -45496,7 +45495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>160</v>
       </c>
@@ -45669,7 +45668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>161</v>
       </c>
@@ -45842,7 +45841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>162</v>
       </c>
@@ -46015,7 +46014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>163</v>
       </c>
@@ -46188,7 +46187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>164</v>
       </c>
@@ -46361,7 +46360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>165</v>
       </c>
@@ -46534,7 +46533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>166</v>
       </c>
@@ -46707,7 +46706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>167</v>
       </c>
@@ -46880,7 +46879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>168</v>
       </c>
@@ -47053,7 +47052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>169</v>
       </c>
@@ -47226,7 +47225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>170</v>
       </c>
@@ -47399,7 +47398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>171</v>
       </c>
@@ -47572,7 +47571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>172</v>
       </c>
@@ -47745,7 +47744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>173</v>
       </c>
@@ -47918,7 +47917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>174</v>
       </c>
@@ -48091,7 +48090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>175</v>
       </c>
@@ -48264,7 +48263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>176</v>
       </c>
@@ -48437,7 +48436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>177</v>
       </c>
@@ -48610,7 +48609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>178</v>
       </c>
@@ -48783,7 +48782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>179</v>
       </c>
@@ -48956,7 +48955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>180</v>
       </c>
@@ -49129,7 +49128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>181</v>
       </c>
@@ -49302,7 +49301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>182</v>
       </c>
@@ -49475,7 +49474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
         <v>183</v>
       </c>
@@ -49648,7 +49647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
         <v>184</v>
       </c>
@@ -49821,7 +49820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
         <v>185</v>
       </c>
@@ -49994,7 +49993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>186</v>
       </c>
@@ -50167,7 +50166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
         <v>187</v>
       </c>
@@ -50340,7 +50339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>188</v>
       </c>
@@ -50513,7 +50512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
         <v>39</v>
       </c>
@@ -50686,7 +50685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
         <v>39</v>
       </c>
@@ -50859,7 +50858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
         <v>189</v>
       </c>
@@ -51032,7 +51031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
         <v>39</v>
       </c>
@@ -51205,7 +51204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A211" s="4" t="s">
         <v>190</v>
       </c>
@@ -51378,7 +51377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
         <v>191</v>
       </c>
@@ -51551,7 +51550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A213" s="4" t="s">
         <v>192</v>
       </c>
@@ -51724,7 +51723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
         <v>39</v>
       </c>
@@ -51897,7 +51896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
         <v>193</v>
       </c>
@@ -52070,7 +52069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
         <v>194</v>
       </c>
@@ -52243,7 +52242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A217" s="4" t="s">
         <v>195</v>
       </c>
@@ -52416,7 +52415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A218" s="4" t="s">
         <v>196</v>
       </c>
@@ -52589,7 +52588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
         <v>197</v>
       </c>
@@ -52762,7 +52761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A220" s="4" t="s">
         <v>198</v>
       </c>
@@ -52935,7 +52934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A221" s="4" t="s">
         <v>199</v>
       </c>
@@ -53108,7 +53107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
         <v>200</v>
       </c>
@@ -53281,7 +53280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
         <v>201</v>
       </c>
@@ -53454,7 +53453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
         <v>202</v>
       </c>
@@ -53627,7 +53626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A225" s="4" t="s">
         <v>203</v>
       </c>
@@ -53800,7 +53799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A226" s="4" t="s">
         <v>204</v>
       </c>
@@ -53973,7 +53972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A227" s="4" t="s">
         <v>205</v>
       </c>
@@ -54146,7 +54145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A228" s="4" t="s">
         <v>206</v>
       </c>
@@ -54319,7 +54318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A229" s="4" t="s">
         <v>207</v>
       </c>
@@ -54492,7 +54491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
         <v>208</v>
       </c>
@@ -54665,7 +54664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
         <v>209</v>
       </c>
@@ -54838,7 +54837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A232" s="4" t="s">
         <v>210</v>
       </c>
@@ -55011,7 +55010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
         <v>211</v>
       </c>
@@ -55184,7 +55183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
         <v>212</v>
       </c>
@@ -55357,7 +55356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
         <v>39</v>
       </c>
@@ -55530,7 +55529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
         <v>213</v>
       </c>
@@ -55703,7 +55702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
         <v>214</v>
       </c>
@@ -55876,7 +55875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
         <v>39</v>
       </c>
@@ -56049,7 +56048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
         <v>215</v>
       </c>
@@ -56222,7 +56221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
         <v>39</v>
       </c>
@@ -56395,7 +56394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A241" s="4" t="s">
         <v>216</v>
       </c>
@@ -56568,7 +56567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A242" s="4" t="s">
         <v>217</v>
       </c>
@@ -56741,7 +56740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A243" s="4" t="s">
         <v>39</v>
       </c>
@@ -56914,7 +56913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A244" s="4" t="s">
         <v>39</v>
       </c>
@@ -57087,7 +57086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A245" s="4" t="s">
         <v>218</v>
       </c>
@@ -57260,7 +57259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A246" s="4" t="s">
         <v>219</v>
       </c>
@@ -57433,7 +57432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
         <v>220</v>
       </c>
@@ -57606,7 +57605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
         <v>221</v>
       </c>
@@ -57779,7 +57778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A249" s="4" t="s">
         <v>222</v>
       </c>
@@ -57952,7 +57951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A250" s="4" t="s">
         <v>223</v>
       </c>
@@ -58125,7 +58124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A251" s="4" t="s">
         <v>224</v>
       </c>
@@ -58298,7 +58297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
         <v>225</v>
       </c>
@@ -58471,7 +58470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A253" s="4" t="s">
         <v>226</v>
       </c>
@@ -58644,7 +58643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
         <v>227</v>
       </c>
@@ -58817,7 +58816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A255" s="4" t="s">
         <v>228</v>
       </c>
@@ -58990,7 +58989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
         <v>229</v>
       </c>
@@ -59163,7 +59162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A257" s="4" t="s">
         <v>230</v>
       </c>
@@ -59336,7 +59335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A258" s="4" t="s">
         <v>231</v>
       </c>
@@ -59509,7 +59508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A259" s="4" t="s">
         <v>232</v>
       </c>
@@ -59682,7 +59681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A260" s="4" t="s">
         <v>233</v>
       </c>
@@ -59855,7 +59854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A261" s="4" t="s">
         <v>234</v>
       </c>
@@ -60028,7 +60027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A262" s="4" t="s">
         <v>235</v>
       </c>
@@ -60201,7 +60200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A263" s="4" t="s">
         <v>236</v>
       </c>
@@ -60374,7 +60373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A264" s="4" t="s">
         <v>237</v>
       </c>
@@ -60547,7 +60546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A265" s="4" t="s">
         <v>238</v>
       </c>
@@ -60720,7 +60719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A266" s="4" t="s">
         <v>239</v>
       </c>
@@ -60893,7 +60892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A267" s="4" t="s">
         <v>240</v>
       </c>
@@ -61066,7 +61065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
         <v>241</v>
       </c>
@@ -61239,7 +61238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A269" s="4" t="s">
         <v>242</v>
       </c>
@@ -61412,7 +61411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A270" s="4" t="s">
         <v>243</v>
       </c>
@@ -61585,7 +61584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A271" s="4" t="s">
         <v>244</v>
       </c>
@@ -61758,7 +61757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A272" s="4" t="s">
         <v>245</v>
       </c>
@@ -61931,7 +61930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A273" s="4" t="s">
         <v>246</v>
       </c>
@@ -62104,7 +62103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A274" s="4" t="s">
         <v>247</v>
       </c>
@@ -62277,7 +62276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A275" s="4" t="s">
         <v>248</v>
       </c>
@@ -62450,7 +62449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A276" s="4" t="s">
         <v>249</v>
       </c>
@@ -62623,7 +62622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A277" s="4" t="s">
         <v>250</v>
       </c>
@@ -62796,7 +62795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A278" s="4" t="s">
         <v>251</v>
       </c>
@@ -62969,7 +62968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A279" s="4" t="s">
         <v>252</v>
       </c>
@@ -63142,7 +63141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A280" s="4" t="s">
         <v>253</v>
       </c>
@@ -63315,7 +63314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A281" s="4" t="s">
         <v>254</v>
       </c>
@@ -63488,7 +63487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A282" s="4" t="s">
         <v>255</v>
       </c>
@@ -63661,7 +63660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A283" s="4" t="s">
         <v>256</v>
       </c>
@@ -63834,7 +63833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
         <v>257</v>
       </c>
@@ -64007,7 +64006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
         <v>258</v>
       </c>
@@ -64180,7 +64179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>259</v>
       </c>
@@ -64353,7 +64352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
         <v>260</v>
       </c>
@@ -64526,7 +64525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
         <v>261</v>
       </c>
@@ -64699,7 +64698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A289" s="4" t="s">
         <v>262</v>
       </c>
@@ -64872,7 +64871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
         <v>263</v>
       </c>
@@ -65045,7 +65044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
         <v>264</v>
       </c>
@@ -65218,7 +65217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A292" s="4" t="s">
         <v>265</v>
       </c>
@@ -65391,7 +65390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A293" s="4" t="s">
         <v>266</v>
       </c>
@@ -65564,7 +65563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
         <v>267</v>
       </c>
@@ -65737,7 +65736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A295" s="4" t="s">
         <v>268</v>
       </c>
@@ -65910,7 +65909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
         <v>269</v>
       </c>
@@ -66083,7 +66082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A297" s="4" t="s">
         <v>270</v>
       </c>
@@ -66256,7 +66255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
         <v>271</v>
       </c>
@@ -66429,7 +66428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
         <v>272</v>
       </c>
@@ -66602,7 +66601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A300" s="4" t="s">
         <v>273</v>
       </c>
@@ -66775,7 +66774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A301" s="4" t="s">
         <v>274</v>
       </c>
@@ -66948,7 +66947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
         <v>275</v>
       </c>
@@ -67121,7 +67120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A303" s="4" t="s">
         <v>276</v>
       </c>
@@ -67294,7 +67293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>277</v>
       </c>
@@ -67467,7 +67466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A305" s="4" t="s">
         <v>278</v>
       </c>
@@ -67640,7 +67639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
         <v>279</v>
       </c>
@@ -67813,7 +67812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A307" s="4" t="s">
         <v>280</v>
       </c>
@@ -67986,7 +67985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A308" s="4" t="s">
         <v>281</v>
       </c>
@@ -68159,7 +68158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A309" s="4" t="s">
         <v>282</v>
       </c>
@@ -68332,7 +68331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A310" s="4" t="s">
         <v>283</v>
       </c>
@@ -68505,7 +68504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A311" s="4" t="s">
         <v>284</v>
       </c>
@@ -68678,7 +68677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A312" s="4" t="s">
         <v>285</v>
       </c>
@@ -68851,7 +68850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A313" s="4" t="s">
         <v>286</v>
       </c>
@@ -69024,7 +69023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
         <v>287</v>
       </c>
@@ -69197,7 +69196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A315" s="4" t="s">
         <v>288</v>
       </c>
@@ -69370,7 +69369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A316" s="4" t="s">
         <v>289</v>
       </c>
@@ -69543,7 +69542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A317" s="4" t="s">
         <v>290</v>
       </c>
@@ -69716,7 +69715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A318" s="4" t="s">
         <v>291</v>
       </c>
@@ -69889,7 +69888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A319" s="4" t="s">
         <v>292</v>
       </c>
@@ -70062,7 +70061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A320" s="4" t="s">
         <v>293</v>
       </c>
@@ -70235,7 +70234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A321" s="4" t="s">
         <v>294</v>
       </c>
@@ -70408,7 +70407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A322" s="4" t="s">
         <v>295</v>
       </c>
@@ -70581,7 +70580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A323" s="4" t="s">
         <v>296</v>
       </c>
@@ -70754,7 +70753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A324" s="4" t="s">
         <v>297</v>
       </c>
@@ -70927,7 +70926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A325" s="4" t="s">
         <v>298</v>
       </c>
@@ -71100,7 +71099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A326" s="4" t="s">
         <v>299</v>
       </c>
@@ -71273,7 +71272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A327" s="4" t="s">
         <v>300</v>
       </c>
@@ -71446,7 +71445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A328" s="4" t="s">
         <v>301</v>
       </c>
@@ -71620,13 +71619,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BE328" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="James R. Ludlow School"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:BE328" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>